<commit_message>
Fleshed out Spring 1 backlog
Built out sprint 1 backlog, waiting for review and others to add input on estimated times
</commit_message>
<xml_diff>
--- a/sprints/sprint1/sprint1_backlog.xlsx
+++ b/sprints/sprint1/sprint1_backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Corley\git\SE2-project-repos-sample\sprints\sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jgain\OneDrive\Documents\School\Spring 2024\SE 2\UWG-SE2-Group5-Myst\sprints\sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9C4265-351C-41A0-89E5-93A08D9C51A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0D3DE7-F04D-49F9-A8B0-E134BB9D5889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Related User Story</t>
   </si>
@@ -64,6 +69,69 @@
   </si>
   <si>
     <t>That User Story</t>
+  </si>
+  <si>
+    <t>Select games that I own/ enjoy</t>
+  </si>
+  <si>
+    <t>Game object, that holds game information</t>
+  </si>
+  <si>
+    <t>UI for selection, searchable, possibily sortable by genres</t>
+  </si>
+  <si>
+    <t>Genre object, which holds list of similar games</t>
+  </si>
+  <si>
+    <t>No database as of now so prexisting local list of games</t>
+  </si>
+  <si>
+    <t>User Validation(might not need since we are the ones uploading games)</t>
+  </si>
+  <si>
+    <t>Testing model/ viewmodel</t>
+  </si>
+  <si>
+    <t>Find recommended/ suggested games</t>
+  </si>
+  <si>
+    <t>UI for recommendation engine, swipe left or right</t>
+  </si>
+  <si>
+    <t>UI element for each recommended game</t>
+  </si>
+  <si>
+    <t>Functionality to save, liked/ dislikes games and genres, based on user's choices</t>
+  </si>
+  <si>
+    <t>Access and view game library</t>
+  </si>
+  <si>
+    <t>UI for game library, show user's owned games</t>
+  </si>
+  <si>
+    <t>UI for ability to select new game user owns</t>
+  </si>
+  <si>
+    <t>UI to display details from game, use image here</t>
+  </si>
+  <si>
+    <t>User/ Profile object, holds user information, list of own games, likes and dislikes</t>
+  </si>
+  <si>
+    <t>Create a profile</t>
+  </si>
+  <si>
+    <t>UI for creating a profile, needs to navigate to UI selection of games</t>
+  </si>
+  <si>
+    <t>UI for basic profile page</t>
+  </si>
+  <si>
+    <t>Library object, which holds maybe a user and then pull the list of games related to that user</t>
+  </si>
+  <si>
+    <t>UI allowing user to edit preferences, undo likes, dislikes</t>
   </si>
 </sst>
 </file>
@@ -145,13 +213,13 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -261,7 +329,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$27:$G$27</c:f>
+              <c:f>Sheet1!$C$28:$G$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1320,27 +1388,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" customWidth="1"/>
-    <col min="2" max="2" width="41.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.44140625" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
@@ -1350,24 +1418,24 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="7" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1390,187 +1458,235 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1579,7 +1695,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1588,7 +1704,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1597,29 +1713,44 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="3">
-        <f>SUM(C3:C26)</f>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
+      <c r="C28" s="3">
+        <f>SUM(C3:C27)</f>
         <v>100</v>
       </c>
-      <c r="D27" s="3">
-        <f t="shared" ref="D27:G27" si="0">SUM(D3:D26)</f>
+      <c r="D28" s="3">
+        <f t="shared" ref="D28:G28" si="0">SUM(D3:D27)</f>
         <v>75</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E28" s="3">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F28" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G28" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Estimates to Sprint 1 Backlog
Added estimates for time on profile creation
</commit_message>
<xml_diff>
--- a/sprints/sprint1/sprint1_backlog.xlsx
+++ b/sprints/sprint1/sprint1_backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/de0b3ea1232571d3/Documents/School/Spring 24/SE2/SE2-Group5-Myst/sprints/sprint1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{3D0D3DE7-F04D-49F9-A8B0-E134BB9D5889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80894E55-3532-4BA9-B0A5-CBC3FCFB72A7}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{3D0D3DE7-F04D-49F9-A8B0-E134BB9D5889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AEC190B-B8B8-4CF6-BABD-032303217DC3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -334,7 +334,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>75</c:v>
@@ -1125,6 +1125,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1391,7 +1395,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1442,9 +1446,7 @@
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1">
-        <v>100</v>
-      </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="2">
         <v>75</v>
       </c>
@@ -1636,7 +1638,9 @@
       <c r="B19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="1">
+        <v>6</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -1647,7 +1651,9 @@
       <c r="B20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1">
+        <v>6</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -1658,7 +1664,9 @@
       <c r="B21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1">
+        <v>6</v>
+      </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -1669,7 +1677,9 @@
       <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" s="1">
+        <v>4</v>
+      </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -1680,7 +1690,9 @@
       <c r="B23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="1"/>
+      <c r="C23" s="1">
+        <v>4</v>
+      </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -1726,7 +1738,7 @@
       <c r="B28" s="1"/>
       <c r="C28" s="3">
         <f>SUM(C3:C27)</f>
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="D28" s="3">
         <f t="shared" ref="D28:G28" si="0">SUM(D3:D27)</f>

</xml_diff>

<commit_message>
Began Implementation on UserCredentials IO
This is the beginning way for how we will be able to access our system
</commit_message>
<xml_diff>
--- a/sprints/sprint1/sprint1_backlog.xlsx
+++ b/sprints/sprint1/sprint1_backlog.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{3D0D3DE7-F04D-49F9-A8B0-E134BB9D5889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C58F9E27-0CED-4D98-827B-C388BB67F750}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -223,13 +223,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1405,7 +1405,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,26 +1416,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1642,13 +1642,13 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="6">
         <v>6</v>
       </c>
       <c r="D19" s="2"/>
@@ -1657,11 +1657,11 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8" t="s">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="6">
         <v>6</v>
       </c>
       <c r="D20" s="2"/>
@@ -1670,11 +1670,11 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8" t="s">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="6">
         <v>6</v>
       </c>
       <c r="D21" s="2"/>
@@ -1683,11 +1683,11 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8" t="s">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="6">
         <v>4</v>
       </c>
       <c r="D22" s="2"/>
@@ -1696,11 +1696,11 @@
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8" t="s">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="6">
         <v>4</v>
       </c>
       <c r="D23" s="2"/>
@@ -1709,9 +1709,9 @@
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1776,7 +1776,7 @@
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="6" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated sprint 1 chart
</commit_message>
<xml_diff>
--- a/sprints/sprint1/sprint1_backlog.xlsx
+++ b/sprints/sprint1/sprint1_backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tl00162\Documents\GitHub\UWG-SE2-Group5-Myst\sprints\sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/de0b3ea1232571d3/Documents/School/Spring 24/SE2/SE2-Group5-Myst/sprints/sprint1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6266B2C-8674-42E1-98D4-9E622DE79225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{F6266B2C-8674-42E1-98D4-9E622DE79225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC8F02A7-DAEF-48DF-9338-94BD5E3CC4C4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25005" yWindow="2400" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -336,7 +347,7 @@
                   <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1124,10 +1135,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1394,7 +1401,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="E6:F6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,9 +1468,7 @@
       <c r="C4" s="1">
         <v>6</v>
       </c>
-      <c r="D4" s="2">
-        <v>6</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1477,7 +1482,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1492,7 +1497,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1507,7 +1512,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1568,9 +1573,7 @@
       <c r="C11" s="1">
         <v>4</v>
       </c>
-      <c r="D11" s="2">
-        <v>4</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1583,9 +1586,7 @@
       <c r="C12" s="1">
         <v>4</v>
       </c>
-      <c r="D12" s="2">
-        <v>4</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1598,9 +1599,7 @@
       <c r="C13" s="1">
         <v>2</v>
       </c>
-      <c r="D13" s="2">
-        <v>2</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1615,9 +1614,7 @@
       <c r="C14" s="1">
         <v>6</v>
       </c>
-      <c r="D14" s="2">
-        <v>6</v>
-      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1630,9 +1627,7 @@
       <c r="C15" s="1">
         <v>6</v>
       </c>
-      <c r="D15" s="2">
-        <v>6</v>
-      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1645,9 +1640,7 @@
       <c r="C16" s="1">
         <v>4</v>
       </c>
-      <c r="D16" s="2">
-        <v>4</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1660,9 +1653,7 @@
       <c r="C17" s="1">
         <v>4</v>
       </c>
-      <c r="D17" s="2">
-        <v>4</v>
-      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1675,9 +1666,7 @@
       <c r="C18" s="1">
         <v>4</v>
       </c>
-      <c r="D18" s="2">
-        <v>4</v>
-      </c>
+      <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1692,9 +1681,7 @@
       <c r="C19" s="6">
         <v>6</v>
       </c>
-      <c r="D19" s="2">
-        <v>6</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1722,9 +1709,7 @@
       <c r="C21" s="6">
         <v>6</v>
       </c>
-      <c r="D21" s="2">
-        <v>6</v>
-      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1803,7 +1788,7 @@
       </c>
       <c r="D28" s="3">
         <f t="shared" ref="D28:G28" si="0">SUM(D3:D27)</f>
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="E28" s="3">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Updating Sprint 1 burndown
</commit_message>
<xml_diff>
--- a/sprints/sprint1/sprint1_backlog.xlsx
+++ b/sprints/sprint1/sprint1_backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jgain\OneDrive\Documents\School\Spring 2024\UWG-SE2-Group5-Myst\sprints\sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AE70B9-4D70-4D13-A608-EBD5393F7F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF0D730-A6C0-4C42-820F-A5C855B4C900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>Related User Story</t>
   </si>
@@ -128,9 +128,6 @@
     <t>UI allowing user to edit preferences, undo likes, dislikes</t>
   </si>
   <si>
-    <t>Genre enum, which holds list of similar games</t>
-  </si>
-  <si>
     <t>Jeffrey</t>
   </si>
   <si>
@@ -141,6 +138,24 @@
   </si>
   <si>
     <t>Mystiverse page</t>
+  </si>
+  <si>
+    <t>Genre enum</t>
+  </si>
+  <si>
+    <t>Create ActiveUser, storing current user</t>
+  </si>
+  <si>
+    <t>Create Profile Attributes to hold more user info</t>
+  </si>
+  <si>
+    <t>Designing Profile SubPages( Edit Preferences, Edit Profile, Settings Profile)</t>
+  </si>
+  <si>
+    <t>Creating subPages viewmodel</t>
+  </si>
+  <si>
+    <t>Testing viewmodel of subpages</t>
   </si>
 </sst>
 </file>
@@ -345,24 +360,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$30:$G$30</c:f>
+              <c:f>Sheet1!$C$34:$G$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>95</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>87</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1404,10 +1419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1480,8 +1495,12 @@
       <c r="E4" s="2">
         <v>6</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="F4" s="2">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
@@ -1497,13 +1516,17 @@
       <c r="E5" s="2">
         <v>1</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -1514,13 +1537,17 @@
       <c r="E6" s="2">
         <v>1</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
@@ -1531,8 +1558,12 @@
       <c r="E7" s="2">
         <v>1</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
@@ -1548,8 +1579,12 @@
       <c r="E8" s="2">
         <v>0</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
@@ -1584,19 +1619,33 @@
       <c r="E10" s="2">
         <v>2</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="C11" s="1">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2">
+        <v>6</v>
+      </c>
+      <c r="F11" s="2">
+        <v>6</v>
+      </c>
+      <c r="G11" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
@@ -1612,13 +1661,17 @@
       <c r="E12" s="2">
         <v>0</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1">
         <v>6</v>
@@ -1629,8 +1682,12 @@
       <c r="E13" s="2">
         <v>2</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
@@ -1646,8 +1703,12 @@
       <c r="E14" s="2">
         <v>2</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
@@ -1663,7 +1724,9 @@
       <c r="E15" s="2">
         <v>1</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1682,8 +1745,12 @@
       <c r="E16" s="2">
         <v>3</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -1733,8 +1800,12 @@
       <c r="E19" s="2">
         <v>2</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
@@ -1750,8 +1821,12 @@
       <c r="E20" s="2">
         <v>4</v>
       </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
@@ -1769,8 +1844,12 @@
       <c r="E21" s="2">
         <v>1</v>
       </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
@@ -1786,8 +1865,12 @@
       <c r="E22" s="2">
         <v>1</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
@@ -1803,8 +1886,12 @@
       <c r="E23" s="2">
         <v>6</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
@@ -1820,8 +1907,12 @@
       <c r="E24" s="2">
         <v>1</v>
       </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
@@ -1837,79 +1928,173 @@
       <c r="E25" s="2">
         <v>4</v>
       </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="B26" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="6">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2">
+        <v>2</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="6">
+        <v>3</v>
+      </c>
+      <c r="D27" s="2">
+        <v>3</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="6">
+        <v>10</v>
+      </c>
+      <c r="D28" s="2">
+        <v>6</v>
+      </c>
+      <c r="E28" s="2">
+        <v>4</v>
+      </c>
+      <c r="F28" s="2">
+        <v>2</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="6">
+        <v>6</v>
+      </c>
+      <c r="D29" s="2">
+        <v>3</v>
+      </c>
+      <c r="E29" s="2">
+        <v>2</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="1"/>
-      <c r="C30" s="3">
-        <f>SUM(C3:C29)</f>
-        <v>95</v>
-      </c>
-      <c r="D30" s="3">
-        <f t="shared" ref="D30:G30" si="0">SUM(D3:D29)</f>
-        <v>87</v>
-      </c>
-      <c r="E30" s="3">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="6">
+        <v>10</v>
+      </c>
+      <c r="D30" s="2">
+        <v>7</v>
+      </c>
+      <c r="E30" s="2">
+        <v>4</v>
+      </c>
+      <c r="F30" s="2">
+        <v>3</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="3">
+        <f>SUM(C3:C33)</f>
+        <v>132</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" ref="D34:G34" si="0">SUM(D3:D33)</f>
+        <v>114</v>
+      </c>
+      <c r="E34" s="3">
         <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="F30" s="3">
+        <v>67</v>
+      </c>
+      <c r="F34" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G30" s="3">
+        <v>18</v>
+      </c>
+      <c r="G34" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
-        <v>31</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating burndown sprint1 chart
</commit_message>
<xml_diff>
--- a/sprints/sprint1/sprint1_backlog.xlsx
+++ b/sprints/sprint1/sprint1_backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jgain\OneDrive\Documents\School\Spring 2024\UWG-SE2-Group5-Myst\sprints\sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/de0b3ea1232571d3/Documents/School/Spring 24/SE2/UWG-SE2-Group5-Myst/sprints/sprint1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF0D730-A6C0-4C42-820F-A5C855B4C900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{4EF0D730-A6C0-4C42-820F-A5C855B4C900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B9F5116-CFBB-46A7-AC00-A140F588775D}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -374,10 +374,10 @@
                   <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1421,18 +1421,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.44140625" customWidth="1"/>
-    <col min="2" max="2" width="41.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.42578125" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1449,7 +1449,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1466,7 +1466,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1479,7 +1479,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>12</v>
@@ -1523,7 +1523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>34</v>
@@ -1544,7 +1544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>31</v>
@@ -1565,7 +1565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>14</v>
@@ -1586,7 +1586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>15</v>
@@ -1600,10 +1600,14 @@
       <c r="E9" s="2">
         <v>2</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1626,7 +1630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>33</v>
@@ -1647,7 +1651,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>18</v>
@@ -1668,7 +1672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>32</v>
@@ -1689,7 +1693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>19</v>
@@ -1710,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>15</v>
@@ -1727,9 +1731,11 @@
       <c r="F15" s="2">
         <v>0</v>
       </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -1752,7 +1758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>23</v>
@@ -1766,10 +1772,14 @@
       <c r="E17" s="2">
         <v>5</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F17" s="2">
+        <v>3</v>
+      </c>
+      <c r="G17" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>22</v>
@@ -1783,10 +1793,14 @@
       <c r="E18" s="2">
         <v>4</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F18" s="2">
+        <v>4</v>
+      </c>
+      <c r="G18" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>28</v>
@@ -1807,7 +1821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>15</v>
@@ -1828,7 +1842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>25</v>
       </c>
@@ -1851,7 +1865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6" t="s">
         <v>27</v>
@@ -1872,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6" t="s">
         <v>29</v>
@@ -1893,7 +1907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6" t="s">
         <v>24</v>
@@ -1914,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6" t="s">
         <v>15</v>
@@ -1935,7 +1949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6" t="s">
         <v>35</v>
@@ -1956,7 +1970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6" t="s">
         <v>36</v>
@@ -1977,7 +1991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6" t="s">
         <v>37</v>
@@ -1998,7 +2012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6" t="s">
         <v>38</v>
@@ -2019,7 +2033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6" t="s">
         <v>39</v>
@@ -2040,7 +2054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2049,7 +2063,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2058,7 +2072,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2067,7 +2081,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>8</v>
       </c>
@@ -2085,14 +2099,14 @@
       </c>
       <c r="F34" s="3">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="G34" s="3">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Repackaging to fit server model
</commit_message>
<xml_diff>
--- a/sprints/sprint1/sprint1_backlog.xlsx
+++ b/sprints/sprint1/sprint1_backlog.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{4EF0D730-A6C0-4C42-820F-A5C855B4C900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B9F5116-CFBB-46A7-AC00-A140F588775D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1156,6 +1156,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1422,7 +1426,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>